<commit_message>
Components and latex stuff
</commit_message>
<xml_diff>
--- a/Datasheet/ComponentsNeeded.xlsx
+++ b/Datasheet/ComponentsNeeded.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE59DD72-AD27-45F8-B3F3-C9B3FA2277B3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1E498B0-8947-4099-B259-B354E6308F34}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
   <si>
     <t>Component</t>
   </si>
@@ -247,13 +242,64 @@
   </si>
   <si>
     <t>Units to buy</t>
+  </si>
+  <si>
+    <t>759-9484</t>
+  </si>
+  <si>
+    <t>920-9830</t>
+  </si>
+  <si>
+    <t>686-9381</t>
+  </si>
+  <si>
+    <t>191-4988</t>
+  </si>
+  <si>
+    <t>866-0764</t>
+  </si>
+  <si>
+    <t>768-7893</t>
+  </si>
+  <si>
+    <t>534-4175</t>
+  </si>
+  <si>
+    <t>545-0624</t>
+  </si>
+  <si>
+    <t>742-7859</t>
+  </si>
+  <si>
+    <t>315-1101</t>
+  </si>
+  <si>
+    <t>871-4035</t>
+  </si>
+  <si>
+    <t>500-2376</t>
+  </si>
+  <si>
+    <t>916-3096</t>
+  </si>
+  <si>
+    <t>693-6040P</t>
+  </si>
+  <si>
+    <t>158-562</t>
+  </si>
+  <si>
+    <t>818-4370</t>
+  </si>
+  <si>
+    <t>Product Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +336,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -312,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -320,9 +372,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,29 +656,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M18"/>
+  <dimension ref="A2:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.9453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.89453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.89453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7890625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="8.88671875" style="2"/>
-    <col min="13" max="13" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="12.20703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="8.89453125" style="2"/>
+    <col min="13" max="13" width="11.3125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="18.3" x14ac:dyDescent="0.7">
+      <c r="A2" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -655,7 +713,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -686,7 +747,10 @@
         <v>1095.098</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -713,7 +777,10 @@
         <v>79.400000000000006</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>58</v>
       </c>
@@ -743,7 +810,10 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>57</v>
       </c>
@@ -770,7 +840,10 @@
         <v>110.69999999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -797,7 +870,10 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
@@ -824,7 +900,10 @@
         <v>67.62</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
@@ -851,7 +930,10 @@
         <v>22.49</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
@@ -878,7 +960,10 @@
         <v>84.8</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
@@ -905,7 +990,10 @@
         <v>72.75</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
@@ -932,7 +1020,10 @@
         <v>40.82</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
@@ -962,7 +1053,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -989,7 +1083,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1016,7 +1113,10 @@
         <v>94.350000000000009</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1043,7 +1143,10 @@
         <v>99.28</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>30</v>
       </c>
@@ -1073,7 +1176,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>50</v>
       </c>

</xml_diff>